<commit_message>
Day 2 Product Backlog
</commit_message>
<xml_diff>
--- a/Product_Backlog/ProductBacklog.xlsx
+++ b/Product_Backlog/ProductBacklog.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruthcarnegie\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruthc\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D2C22E-9C9B-4883-9A06-0CFE3A75F6FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="-7140" yWindow="-120" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,9 +97,6 @@
     <t>I can plan a route and visualise the location</t>
   </si>
   <si>
-    <t>add location information to the app</t>
-  </si>
-  <si>
     <t>customise my current live location</t>
   </si>
   <si>
@@ -178,12 +176,15 @@
   </si>
   <si>
     <t xml:space="preserve">I can see options within my budget. </t>
+  </si>
+  <si>
+    <t>Add location information to the app</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -215,7 +216,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,6 +241,12 @@
         <bgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -253,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -275,6 +282,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,15 +504,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -512,7 +521,7 @@
     <col min="3" max="3" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -535,7 +544,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -558,7 +567,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -581,7 +590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -604,7 +613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -627,7 +636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -650,7 +659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -673,12 +682,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>12</v>
@@ -696,7 +705,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
@@ -719,7 +728,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
@@ -742,15 +751,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="D11" s="11">
         <v>6</v>
@@ -765,15 +774,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>44</v>
       </c>
       <c r="D12" s="10">
         <v>3</v>
@@ -788,7 +797,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -808,116 +817,116 @@
         <v>1</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="7" t="s">
+    <row r="14" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="10">
+        <v>9</v>
+      </c>
+      <c r="E14" s="10">
+        <v>7</v>
+      </c>
+      <c r="F14" s="10">
+        <v>2</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="11">
+        <v>6</v>
+      </c>
+      <c r="E15" s="11">
+        <v>6</v>
+      </c>
+      <c r="F15" s="11">
+        <v>2</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="D16" s="7">
+        <v>6</v>
+      </c>
+      <c r="E16" s="7">
+        <v>4</v>
+      </c>
+      <c r="F16" s="7">
+        <v>2</v>
+      </c>
+      <c r="G16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="7">
-        <v>6</v>
-      </c>
-      <c r="E14" s="7">
-        <v>4</v>
-      </c>
-      <c r="F14" s="7">
-        <v>2</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="10"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="10" t="s">
+    </row>
+    <row r="17" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="11">
-        <v>6</v>
-      </c>
-      <c r="E15" s="11">
-        <v>6</v>
-      </c>
-      <c r="F15" s="11">
-        <v>2</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" s="10"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="11">
-        <v>6</v>
-      </c>
-      <c r="E16" s="11">
-        <v>6</v>
-      </c>
-      <c r="F16" s="11">
-        <v>2</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="6" t="s">
+      <c r="D17" s="11">
+        <v>6</v>
+      </c>
+      <c r="E17" s="11">
+        <v>6</v>
+      </c>
+      <c r="F17" s="11">
+        <v>2</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="6">
+      <c r="D18" s="6">
         <v>5</v>
-      </c>
-      <c r="E17" s="6">
-        <v>5</v>
-      </c>
-      <c r="F17" s="6">
-        <v>2</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="6">
-        <v>4</v>
       </c>
       <c r="E18" s="6">
         <v>5</v>
@@ -926,53 +935,53 @@
         <v>2</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D19" s="6">
         <v>4</v>
       </c>
       <c r="E19" s="6">
+        <v>5</v>
+      </c>
+      <c r="F19" s="6">
+        <v>2</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="6">
         <v>4</v>
       </c>
-      <c r="F19" s="6">
-        <v>2</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="6">
-        <v>3</v>
-      </c>
       <c r="E20" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F20" s="6">
         <v>2</v>
       </c>
-      <c r="G20" s="8" t="s">
-        <v>27</v>
+      <c r="G20" s="12" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -980,22 +989,22 @@
         <v>18</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D21" s="10">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E21" s="10">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F21" s="10">
         <v>2</v>
       </c>
-      <c r="G21" s="14" t="s">
-        <v>48</v>
+      <c r="G21" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1003,10 +1012,10 @@
         <v>18</v>
       </c>
       <c r="B22" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="D22" s="10">
         <v>8</v>
@@ -1018,7 +1027,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1026,10 +1035,10 @@
         <v>18</v>
       </c>
       <c r="B23" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>51</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>52</v>
       </c>
       <c r="D23" s="10">
         <v>5</v>
@@ -1041,12 +1050,16 @@
         <v>2</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>27</v>
-      </c>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
     </row>
   </sheetData>
-  <sortState ref="A2:G21">
-    <sortCondition ref="G10"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G23">
+    <sortCondition ref="G17"/>
   </sortState>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>